<commit_message>
HKD Contributor bug fix
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/HKD/HKD_MxContributor.xlsx
+++ b/QuantLibXL/Data2/XLS/HKD/HKD_MxContributor.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="12705" yWindow="-15" windowWidth="12720" windowHeight="12105" activeTab="1"/>
+    <workbookView xWindow="-1290" yWindow="1665" windowWidth="18645" windowHeight="11970" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="General Settings" sheetId="2" r:id="rId1"/>
@@ -1225,6 +1225,8 @@
         <stp>_x000C_HKD6M12X18F=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="AG21" s="7"/>
       </tp>
+    </main>
+    <main first="pldatasource.rtgetrtdserver">
       <tp>
         <v>1.312060199</v>
         <stp/>
@@ -1627,8 +1629,6 @@
 HKDOIS7YD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="AI26" s="7"/>
       </tp>
-    </main>
-    <main first="pldatasource.rtgetrtdserver">
       <tp>
         <v>0.15</v>
         <stp/>
@@ -1781,8 +1781,6 @@
         <stp>_x0008_HKD3M5Y=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="AF25" s="7"/>
       </tp>
-    </main>
-    <main first="pldatasource.rtgetrtdserver">
       <tp>
         <v>1.97</v>
         <stp/>
@@ -2071,6 +2069,8 @@
         <stp>_x0008_HKD1M9M=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="AC17" s="7"/>
       </tp>
+    </main>
+    <main first="pldatasource.rtgetrtdserver">
       <tp>
         <v>1.9</v>
         <stp/>
@@ -2404,14 +2404,47 @@
       <sheetData sheetId="0">
         <row r="7">
           <cell r="D7">
-            <v>22</v>
+            <v>4</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="1">
+        <row r="4">
+          <cell r="M4">
+            <v>5.4299999999999994E-2</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="M5">
+            <v>9.3859999999999985E-2</v>
+          </cell>
+        </row>
         <row r="7">
           <cell r="D7" t="str">
-            <v>HKD1M#0001</v>
+            <v>HKD1M#0000</v>
+          </cell>
+          <cell r="M7">
+            <v>0.24285999999999999</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="M8">
+            <v>0.31935999999999998</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="M9">
+            <v>0.39842</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="M10">
+            <v>0.56054999999999999</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="M11">
+            <v>0.87220999999999993</v>
           </cell>
         </row>
       </sheetData>
@@ -2799,7 +2832,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="55">
-        <v>42279.458032407405</v>
+        <v>42279.477141203701</v>
       </c>
       <c r="E4" s="54"/>
     </row>
@@ -2821,7 +2854,7 @@
       </c>
       <c r="D6" s="56">
         <f>[1]!TriggerCounter</f>
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="E6" s="54"/>
     </row>
@@ -3319,11 +3352,11 @@
       </c>
       <c r="R6" s="9">
         <f>'6M Pricing'!I6*100</f>
-        <v>1.6790870699831355</v>
+        <v>0.54796902249213786</v>
       </c>
       <c r="S6" s="9">
         <f>R6</f>
-        <v>1.6790870699831355</v>
+        <v>0.54796902249213786</v>
       </c>
       <c r="T6" s="97"/>
       <c r="U6" s="8"/>
@@ -3338,12 +3371,12 @@
         <v>HKDSTDOND=</v>
       </c>
       <c r="Z6" s="82">
-        <f>[1]Hibor!$V6</f>
-        <v>0</v>
+        <f>[1]Hibor!$M4</f>
+        <v>5.4299999999999994E-2</v>
       </c>
       <c r="AA6" s="82">
         <f t="shared" ref="AA6:AA29" si="4">Z6</f>
-        <v>0</v>
+        <v>5.4299999999999994E-2</v>
       </c>
       <c r="AB6" s="75" t="s">
         <v>51</v>
@@ -3366,21 +3399,21 @@
       </c>
       <c r="AG6" s="82">
         <f>ABS(_xll.RtGet(SourceAlias,$Q6,BID)-R6)</f>
-        <v>1.1311180469831355</v>
+        <v>5.0786219674137101E-10</v>
       </c>
       <c r="AH6" s="82">
         <f>ABS(_xll.RtGet(SourceAlias,$Q6,ASK)-S6)</f>
-        <v>1.1311180469831355</v>
+        <v>5.0786219674137101E-10</v>
       </c>
       <c r="AI6" s="82"/>
       <c r="AJ6" s="82"/>
       <c r="AK6" s="82">
         <f>ABS(_xll.RtGet(SourceAlias,$Y6,BID)-Z6)</f>
-        <v>5.4299999999999994E-2</v>
+        <v>0</v>
       </c>
       <c r="AL6" s="82">
         <f>ABS(_xll.RtGet(SourceAlias,$Y6,ASK)-AA6)</f>
-        <v>5.4299999999999994E-2</v>
+        <v>0</v>
       </c>
       <c r="AM6" s="34" t="s">
         <v>51</v>
@@ -3454,11 +3487,11 @@
       </c>
       <c r="R7" s="11">
         <f>'6M Pricing'!I7*100</f>
-        <v>1.6749878481790832</v>
+        <v>0.54803030764345129</v>
       </c>
       <c r="S7" s="11">
         <f t="shared" ref="S7:S29" si="7">R7</f>
-        <v>1.6749878481790832</v>
+        <v>0.54803030764345129</v>
       </c>
       <c r="T7" s="98"/>
       <c r="U7" s="10"/>
@@ -3473,12 +3506,12 @@
         <v>HKDSTD1WD=</v>
       </c>
       <c r="Z7" s="84">
-        <f>[1]Hibor!$V7</f>
-        <v>0</v>
+        <f>[1]Hibor!$M5</f>
+        <v>9.3859999999999985E-2</v>
       </c>
       <c r="AA7" s="84">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>9.3859999999999985E-2</v>
       </c>
       <c r="AB7" s="75" t="s">
         <v>51</v>
@@ -3501,21 +3534,21 @@
       </c>
       <c r="AG7" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$Q7,BID)-R7)</f>
-        <v>1.1269575401790832</v>
+        <v>3.5654867946988134E-10</v>
       </c>
       <c r="AH7" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$Q7,ASK)-S7)</f>
-        <v>1.1269575401790832</v>
+        <v>3.5654867946988134E-10</v>
       </c>
       <c r="AI7" s="84"/>
       <c r="AJ7" s="84"/>
       <c r="AK7" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$Y7,BID)-Z7)</f>
-        <v>9.3859999999999985E-2</v>
+        <v>0</v>
       </c>
       <c r="AL7" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$Y7,ASK)-AA7)</f>
-        <v>9.3859999999999985E-2</v>
+        <v>0</v>
       </c>
       <c r="AM7" s="34" t="s">
         <v>51</v>
@@ -3588,11 +3621,11 @@
       </c>
       <c r="R8" s="11">
         <f>'6M Pricing'!I8*100</f>
-        <v>1.6683833065945866</v>
+        <v>0.54813153550408478</v>
       </c>
       <c r="S8" s="11">
         <f t="shared" si="7"/>
-        <v>1.6683833065945866</v>
+        <v>0.54813153550408478</v>
       </c>
       <c r="T8" s="98"/>
       <c r="U8" s="10"/>
@@ -3623,11 +3656,11 @@
       </c>
       <c r="AG8" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$Q8,BID)-R8)</f>
-        <v>1.1202517705945865</v>
+        <v>4.9591519779568216E-10</v>
       </c>
       <c r="AH8" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$Q8,ASK)-S8)</f>
-        <v>1.1202517705945865</v>
+        <v>4.9591519779568216E-10</v>
       </c>
       <c r="AI8" s="84"/>
       <c r="AJ8" s="84"/>
@@ -3706,11 +3739,11 @@
       </c>
       <c r="R9" s="11">
         <f>'6M Pricing'!I9*100</f>
-        <v>1.6389613010210822</v>
+        <v>0.54851820040111643</v>
       </c>
       <c r="S9" s="11">
         <f t="shared" si="7"/>
-        <v>1.6389613010210822</v>
+        <v>0.54851820040111643</v>
       </c>
       <c r="T9" s="98" t="str">
         <f t="shared" ref="T9:T14" si="8">A9&amp;"D"</f>
@@ -3737,12 +3770,12 @@
         <v>HKDSTD1MD=</v>
       </c>
       <c r="Z9" s="84">
-        <f>[1]Hibor!$V9</f>
-        <v>0</v>
+        <f>[1]Hibor!$M7</f>
+        <v>0.24285999999999999</v>
       </c>
       <c r="AA9" s="84">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>0.24285999999999999</v>
       </c>
       <c r="AB9" s="75" t="s">
         <v>51</v>
@@ -3765,11 +3798,11 @@
       </c>
       <c r="AG9" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$Q9,BID)-R9)</f>
-        <v>1.0904431000210821</v>
+        <v>5.9888360937065954E-10</v>
       </c>
       <c r="AH9" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$Q9,ASK)-S9)</f>
-        <v>1.0904431000210821</v>
+        <v>5.9888360937065954E-10</v>
       </c>
       <c r="AI9" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$U9,BID)-V9)</f>
@@ -3781,11 +3814,11 @@
       </c>
       <c r="AK9" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$Y9,BID)-Z9)</f>
-        <v>0.24285999999999999</v>
+        <v>0</v>
       </c>
       <c r="AL9" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$Y9,ASK)-AA9)</f>
-        <v>0.24285999999999999</v>
+        <v>0</v>
       </c>
       <c r="AM9" s="34" t="s">
         <v>51</v>
@@ -3834,11 +3867,11 @@
       </c>
       <c r="R10" s="11">
         <f>'6M Pricing'!I10*100</f>
-        <v>1.5320304902725597</v>
+        <v>0.54978770972757296</v>
       </c>
       <c r="S10" s="11">
         <f t="shared" si="7"/>
-        <v>1.5320304902725597</v>
+        <v>0.54978770972757296</v>
       </c>
       <c r="T10" s="98" t="str">
         <f t="shared" si="8"/>
@@ -3865,12 +3898,12 @@
         <v>HKDSTD2MD=</v>
       </c>
       <c r="Z10" s="84">
-        <f>[1]Hibor!$V10</f>
-        <v>0</v>
+        <f>[1]Hibor!$M8</f>
+        <v>0.31935999999999998</v>
       </c>
       <c r="AA10" s="84">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>0.31935999999999998</v>
       </c>
       <c r="AB10" s="75" t="s">
         <v>51</v>
@@ -3881,11 +3914,11 @@
       <c r="AF10" s="84"/>
       <c r="AG10" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$Q10,BID)-R10)</f>
-        <v>0.98224278027255962</v>
+        <v>2.7242708089403322E-10</v>
       </c>
       <c r="AH10" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$Q10,ASK)-S10)</f>
-        <v>0.98224278027255962</v>
+        <v>2.7242708089403322E-10</v>
       </c>
       <c r="AI10" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$U10,BID)-V10)</f>
@@ -3897,11 +3930,11 @@
       </c>
       <c r="AK10" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$Y10,BID)-Z10)</f>
-        <v>0.31935999999999998</v>
+        <v>0</v>
       </c>
       <c r="AL10" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$Y10,ASK)-AA10)</f>
-        <v>0.31935999999999998</v>
+        <v>0</v>
       </c>
       <c r="AM10" s="34" t="s">
         <v>51</v>
@@ -3976,11 +4009,11 @@
       </c>
       <c r="R11" s="11">
         <f>'6M Pricing'!I11*100</f>
-        <v>1.3768217292016267</v>
+        <v>0.55155003031810879</v>
       </c>
       <c r="S11" s="11">
         <f t="shared" si="7"/>
-        <v>1.3768217292016267</v>
+        <v>0.55155003031810879</v>
       </c>
       <c r="T11" s="98" t="str">
         <f t="shared" si="8"/>
@@ -4007,12 +4040,12 @@
         <v>HKDSTD3MD=</v>
       </c>
       <c r="Z11" s="84">
-        <f>[1]Hibor!$V11</f>
-        <v>0</v>
+        <f>[1]Hibor!$M9</f>
+        <v>0.39842</v>
       </c>
       <c r="AA11" s="84">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>0.39842</v>
       </c>
       <c r="AB11" s="75" t="s">
         <v>51</v>
@@ -4035,11 +4068,11 @@
       </c>
       <c r="AG11" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$Q11,BID)-R11)</f>
-        <v>0.82527169920162669</v>
+        <v>3.1810876155446977E-10</v>
       </c>
       <c r="AH11" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$Q11,ASK)-S11)</f>
-        <v>0.82527169920162669</v>
+        <v>3.1810876155446977E-10</v>
       </c>
       <c r="AI11" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$U11,BID)-V11)</f>
@@ -4051,11 +4084,11 @@
       </c>
       <c r="AK11" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$Y11,BID)-Z11)</f>
-        <v>0.39842</v>
+        <v>0</v>
       </c>
       <c r="AL11" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$Y11,ASK)-AA11)</f>
-        <v>0.39842</v>
+        <v>0</v>
       </c>
       <c r="AM11" s="34" t="s">
         <v>51</v>
@@ -4115,11 +4148,11 @@
       </c>
       <c r="R12" s="11">
         <f>'6M Pricing'!I12*100</f>
-        <v>1.1495185398286245</v>
+        <v>0.55407809823303089</v>
       </c>
       <c r="S12" s="11">
         <f t="shared" si="7"/>
-        <v>1.1495185398286245</v>
+        <v>0.55407809823303089</v>
       </c>
       <c r="T12" s="98" t="str">
         <f t="shared" si="8"/>
@@ -4156,11 +4189,11 @@
       </c>
       <c r="AG12" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$Q12,BID)-R12)</f>
-        <v>0.59544044182862454</v>
+        <v>2.3303092788751201E-10</v>
       </c>
       <c r="AH12" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$Q12,ASK)-S12)</f>
-        <v>0.59544044182862454</v>
+        <v>2.3303092788751201E-10</v>
       </c>
       <c r="AI12" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$U12,BID)-V12)</f>
@@ -4218,11 +4251,11 @@
       </c>
       <c r="R13" s="11">
         <f>'6M Pricing'!I13*100</f>
-        <v>0.85884049460434375</v>
+        <v>0.55727279240825989</v>
       </c>
       <c r="S13" s="11">
         <f t="shared" si="7"/>
-        <v>0.85884049460434375</v>
+        <v>0.55727279240825989</v>
       </c>
       <c r="T13" s="98" t="str">
         <f t="shared" si="8"/>
@@ -4253,11 +4286,11 @@
       <c r="AF13" s="84"/>
       <c r="AG13" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$Q13,BID)-R13)</f>
-        <v>0.30156770260434373</v>
+        <v>4.0825987035475464E-10</v>
       </c>
       <c r="AH13" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$Q13,ASK)-S13)</f>
-        <v>0.30156770260434373</v>
+        <v>4.0825987035475464E-10</v>
       </c>
       <c r="AI13" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$U13,BID)-V13)</f>
@@ -4341,11 +4374,11 @@
       </c>
       <c r="R14" s="11">
         <f>'6M Pricing'!I14*100</f>
-        <v>0.52952602541179272</v>
+        <v>0.56086587043454339</v>
       </c>
       <c r="S14" s="11">
         <f t="shared" si="7"/>
-        <v>0.52952602541179272</v>
+        <v>0.56086587043454339</v>
       </c>
       <c r="T14" s="98" t="str">
         <f t="shared" si="8"/>
@@ -4372,12 +4405,12 @@
         <v>HKDSTD6MD=</v>
       </c>
       <c r="Z14" s="84">
-        <f>[1]Hibor!$V12</f>
-        <v>0</v>
+        <f>[1]Hibor!$M10</f>
+        <v>0.56054999999999999</v>
       </c>
       <c r="AA14" s="84">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>0.56054999999999999</v>
       </c>
       <c r="AB14" s="75" t="s">
         <v>51</v>
@@ -4400,11 +4433,11 @@
       </c>
       <c r="AG14" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$Q14,BID)-R14)</f>
-        <v>3.1339844588207266E-2</v>
+        <v>4.3454340126203306E-10</v>
       </c>
       <c r="AH14" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$Q14,ASK)-S14)</f>
-        <v>3.1339844588207266E-2</v>
+        <v>4.3454340126203306E-10</v>
       </c>
       <c r="AI14" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$U14,BID)-V14)</f>
@@ -4416,11 +4449,11 @@
       </c>
       <c r="AK14" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$Y14,BID)-Z14)</f>
-        <v>0.56054999999999999</v>
+        <v>0</v>
       </c>
       <c r="AL14" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$Y14,ASK)-AA14)</f>
-        <v>0.56054999999999999</v>
+        <v>0</v>
       </c>
       <c r="AM14" s="34" t="s">
         <v>51</v>
@@ -4466,11 +4499,11 @@
       </c>
       <c r="R15" s="11">
         <f>'6M Pricing'!I15*100</f>
-        <v>-3.2640991011183208E-2</v>
+        <v>0.57186023228693061</v>
       </c>
       <c r="S15" s="11">
         <f t="shared" si="7"/>
-        <v>-3.2640991011183208E-2</v>
+        <v>0.57186023228693061</v>
       </c>
       <c r="T15" s="98"/>
       <c r="U15" s="10"/>
@@ -4487,11 +4520,11 @@
       <c r="AF15" s="84"/>
       <c r="AG15" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$Q15,BID)-R15)</f>
-        <v>0.60450122401118322</v>
+        <v>7.1306938131954212E-10</v>
       </c>
       <c r="AH15" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$Q15,ASK)-S15)</f>
-        <v>0.60450122401118322</v>
+        <v>7.1306938131954212E-10</v>
       </c>
       <c r="AI15" s="84"/>
       <c r="AJ15" s="84"/>
@@ -4539,11 +4572,11 @@
       </c>
       <c r="R16" s="11">
         <f>'6M Pricing'!I16*100</f>
-        <v>1.0397867244255034E-2</v>
+        <v>0.60837988335763782</v>
       </c>
       <c r="S16" s="11">
         <f t="shared" si="7"/>
-        <v>1.0397867244255034E-2</v>
+        <v>0.60837988335763782</v>
       </c>
       <c r="T16" s="98"/>
       <c r="U16" s="10"/>
@@ -4560,11 +4593,11 @@
       <c r="AF16" s="84"/>
       <c r="AG16" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$Q16,BID)-R16)</f>
-        <v>0.59798201575574494</v>
+        <v>3.5763780825703861E-10</v>
       </c>
       <c r="AH16" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$Q16,ASK)-S16)</f>
-        <v>0.59798201575574494</v>
+        <v>3.5763780825703861E-10</v>
       </c>
       <c r="AI16" s="84"/>
       <c r="AJ16" s="84"/>
@@ -4638,11 +4671,11 @@
       </c>
       <c r="R17" s="11">
         <f>'6M Pricing'!I17*100</f>
-        <v>-9.5927591562247226E-4</v>
+        <v>0.66332620453451585</v>
       </c>
       <c r="S17" s="11">
         <f t="shared" si="7"/>
-        <v>-9.5927591562247226E-4</v>
+        <v>0.66332620453451585</v>
       </c>
       <c r="T17" s="98" t="str">
         <f>A17&amp;"D"</f>
@@ -4685,11 +4718,11 @@
       </c>
       <c r="AG17" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$Q17,BID)-R17)</f>
-        <v>0.66428548091562245</v>
+        <v>4.6548409571300908E-10</v>
       </c>
       <c r="AH17" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$Q17,ASK)-S17)</f>
-        <v>0.66428548091562245</v>
+        <v>4.6548409571300908E-10</v>
       </c>
       <c r="AI17" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$U17,BID)-V17)</f>
@@ -4745,11 +4778,11 @@
       </c>
       <c r="R18" s="11">
         <f>'6M Pricing'!I18*100</f>
-        <v>6.0833558678996893E-4</v>
+        <v>0.7079619863913964</v>
       </c>
       <c r="S18" s="11">
         <f t="shared" si="7"/>
-        <v>6.0833558678996893E-4</v>
+        <v>0.7079619863913964</v>
       </c>
       <c r="T18" s="98"/>
       <c r="U18" s="10"/>
@@ -4766,11 +4799,11 @@
       <c r="AF18" s="84"/>
       <c r="AG18" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$Q18,BID)-R18)</f>
-        <v>0.70735364141321</v>
+        <v>9.39139643829634E-9</v>
       </c>
       <c r="AH18" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$Q18,ASK)-S18)</f>
-        <v>0.70735364141321</v>
+        <v>9.39139643829634E-9</v>
       </c>
       <c r="AI18" s="84"/>
       <c r="AJ18" s="84"/>
@@ -4818,11 +4851,11 @@
       </c>
       <c r="R19" s="11">
         <f>'6M Pricing'!I19*100</f>
-        <v>2.0201377357025947E-3</v>
+        <v>0.74621169541505972</v>
       </c>
       <c r="S19" s="11">
         <f t="shared" si="7"/>
-        <v>2.0201377357025947E-3</v>
+        <v>0.74621169541505972</v>
       </c>
       <c r="T19" s="98"/>
       <c r="U19" s="10"/>
@@ -4839,11 +4872,11 @@
       <c r="AF19" s="84"/>
       <c r="AG19" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$Q19,BID)-R19)</f>
-        <v>0.7441915852642973</v>
+        <v>2.7584940220926057E-8</v>
       </c>
       <c r="AH19" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$Q19,ASK)-S19)</f>
-        <v>0.7441915852642973</v>
+        <v>2.7584940220926057E-8</v>
       </c>
       <c r="AI19" s="84"/>
       <c r="AJ19" s="84"/>
@@ -4919,11 +4952,11 @@
       </c>
       <c r="R20" s="11">
         <f>'6M Pricing'!I20*100</f>
-        <v>-3.5271658559814798E-3</v>
+        <v>0.78265007100070016</v>
       </c>
       <c r="S20" s="11">
         <f t="shared" si="7"/>
-        <v>-3.5271658559814798E-3</v>
+        <v>0.78265007100070016</v>
       </c>
       <c r="T20" s="98" t="str">
         <f t="shared" ref="T20:T29" si="13">A20&amp;"D"</f>
@@ -4950,12 +4983,12 @@
         <v>HKDSTD1YD=</v>
       </c>
       <c r="Z20" s="84">
-        <f>[1]Hibor!$V14</f>
-        <v>0</v>
+        <f>[1]Hibor!$M11</f>
+        <v>0.87220999999999993</v>
       </c>
       <c r="AA20" s="84">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>0.87220999999999993</v>
       </c>
       <c r="AB20" s="75" t="s">
         <v>51</v>
@@ -4978,11 +5011,11 @@
       </c>
       <c r="AG20" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$Q20,BID)-R20)</f>
-        <v>0.7861771978559815</v>
+        <v>3.9000700113867026E-8</v>
       </c>
       <c r="AH20" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$Q20,ASK)-S20)</f>
-        <v>0.7861771978559815</v>
+        <v>3.9000700113867026E-8</v>
       </c>
       <c r="AI20" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$U20,BID)-V20)</f>
@@ -4994,11 +5027,11 @@
       </c>
       <c r="AK20" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$Y20,BID)-Z20)</f>
-        <v>0.87220999999999993</v>
+        <v>0</v>
       </c>
       <c r="AL20" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$Y20,ASK)-AA20)</f>
-        <v>0.87220999999999993</v>
+        <v>0</v>
       </c>
       <c r="AM20" s="34" t="s">
         <v>51</v>
@@ -5058,11 +5091,11 @@
       </c>
       <c r="R21" s="11">
         <f>'6M Pricing'!I21*100</f>
-        <v>-7.4190239538407044E-4</v>
+        <v>1.0544016682418924</v>
       </c>
       <c r="S21" s="11">
         <f t="shared" si="7"/>
-        <v>-7.4190239538407044E-4</v>
+        <v>1.0544016682418924</v>
       </c>
       <c r="T21" s="98" t="str">
         <f t="shared" si="13"/>
@@ -5099,11 +5132,11 @@
       </c>
       <c r="AG21" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$Q21,BID)-R21)</f>
-        <v>1.055144016395384</v>
+        <v>4.4575810753677558E-7</v>
       </c>
       <c r="AH21" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$Q21,ASK)-S21)</f>
-        <v>1.055144016395384</v>
+        <v>4.4575810753677558E-7</v>
       </c>
       <c r="AI21" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$U21,BID)-V21)</f>
@@ -5187,11 +5220,11 @@
       </c>
       <c r="R22" s="11">
         <f>'6M Pricing'!I22*100</f>
-        <v>1.2203135604930689E-2</v>
+        <v>1.3120611247400937</v>
       </c>
       <c r="S22" s="11">
         <f t="shared" si="7"/>
-        <v>1.2203135604930689E-2</v>
+        <v>1.3120611247400937</v>
       </c>
       <c r="T22" s="98" t="str">
         <f t="shared" si="13"/>
@@ -5246,11 +5279,11 @@
       </c>
       <c r="AG22" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$Q22,BID)-R22)</f>
-        <v>1.2998570633950695</v>
+        <v>9.2574009369350563E-7</v>
       </c>
       <c r="AH22" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$Q22,ASK)-S22)</f>
-        <v>1.2998570633950695</v>
+        <v>9.2574009369350563E-7</v>
       </c>
       <c r="AI22" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$U22,BID)-V22)</f>
@@ -5341,11 +5374,11 @@
       </c>
       <c r="R23" s="11">
         <f>'6M Pricing'!I23*100</f>
-        <v>-0.38335737215488042</v>
+        <v>1.0653784599269873</v>
       </c>
       <c r="S23" s="11">
         <f t="shared" si="7"/>
-        <v>-0.38335737215488042</v>
+        <v>1.0653784599269873</v>
       </c>
       <c r="T23" s="98" t="str">
         <f t="shared" si="13"/>
@@ -5400,11 +5433,11 @@
       </c>
       <c r="AG23" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$Q23,BID)-R23)</f>
-        <v>1.4487294771548804</v>
+        <v>6.3549269873064418E-6</v>
       </c>
       <c r="AH23" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$Q23,ASK)-S23)</f>
-        <v>1.4487294771548804</v>
+        <v>6.3549269873064418E-6</v>
       </c>
       <c r="AI23" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$U23,BID)-V23)</f>
@@ -5495,11 +5528,11 @@
       </c>
       <c r="R24" s="11">
         <f>'6M Pricing'!I24*100</f>
-        <v>-0.64461427424037776</v>
+        <v>1.1360400410021656</v>
       </c>
       <c r="S24" s="11">
         <f t="shared" si="7"/>
-        <v>-0.64461427424037776</v>
+        <v>1.1360400410021656</v>
       </c>
       <c r="T24" s="98" t="str">
         <f t="shared" si="13"/>
@@ -5554,11 +5587,11 @@
       </c>
       <c r="AG24" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$Q24,BID)-R24)</f>
-        <v>1.7806448262403778</v>
+        <v>9.4890021655746892E-6</v>
       </c>
       <c r="AH24" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$Q24,ASK)-S24)</f>
-        <v>1.7806448262403778</v>
+        <v>9.4890021655746892E-6</v>
       </c>
       <c r="AI24" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$U24,BID)-V24)</f>
@@ -5649,11 +5682,11 @@
       </c>
       <c r="R25" s="11">
         <f>'6M Pricing'!I25*100</f>
-        <v>-0.8004884079265423</v>
+        <v>1.1780535604938696</v>
       </c>
       <c r="S25" s="11">
         <f t="shared" si="7"/>
-        <v>-0.8004884079265423</v>
+        <v>1.1780535604938696</v>
       </c>
       <c r="T25" s="98" t="str">
         <f t="shared" si="13"/>
@@ -5708,11 +5741,11 @@
       </c>
       <c r="AG25" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$Q25,BID)-R25)</f>
-        <v>1.9785306179265425</v>
+        <v>1.1350493869466405E-5</v>
       </c>
       <c r="AH25" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$Q25,ASK)-S25)</f>
-        <v>1.9785306179265425</v>
+        <v>1.1350493869466405E-5</v>
       </c>
       <c r="AI25" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$U25,BID)-V25)</f>
@@ -5803,11 +5836,11 @@
       </c>
       <c r="R26" s="11">
         <f>'6M Pricing'!I26*100</f>
-        <v>-0.97971275502906874</v>
+        <v>1.226237487290244</v>
       </c>
       <c r="S26" s="11">
         <f t="shared" si="7"/>
-        <v>-0.97971275502906874</v>
+        <v>1.226237487290244</v>
       </c>
       <c r="T26" s="98" t="str">
         <f t="shared" si="13"/>
@@ -5862,11 +5895,11 @@
       </c>
       <c r="AG26" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$Q26,BID)-R26)</f>
-        <v>2.2059367590290688</v>
+        <v>1.3483290243865298E-5</v>
       </c>
       <c r="AH26" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$Q26,ASK)-S26)</f>
-        <v>2.2059367590290688</v>
+        <v>1.3483290243865298E-5</v>
       </c>
       <c r="AI26" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$U26,BID)-V26)</f>
@@ -5957,11 +5990,11 @@
       </c>
       <c r="R27" s="11">
         <f>'6M Pricing'!I27*100</f>
-        <v>-1.1145863978438648</v>
+        <v>1.2624128360856059</v>
       </c>
       <c r="S27" s="11">
         <f t="shared" si="7"/>
-        <v>-1.1145863978438648</v>
+        <v>1.2624128360856059</v>
       </c>
       <c r="T27" s="98" t="str">
         <f t="shared" si="13"/>
@@ -6016,11 +6049,11 @@
       </c>
       <c r="AG27" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$Q27,BID)-R27)</f>
-        <v>2.3769841508438647</v>
+        <v>1.5083085605827051E-5</v>
       </c>
       <c r="AH27" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$Q27,ASK)-S27)</f>
-        <v>2.3769841508438647</v>
+        <v>1.5083085605827051E-5</v>
       </c>
       <c r="AI27" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$U27,BID)-V27)</f>
@@ -6111,11 +6144,11 @@
       </c>
       <c r="R28" s="11">
         <f>'6M Pricing'!I28*100</f>
-        <v>-1.166900834583948</v>
+        <v>1.2764220823632126</v>
       </c>
       <c r="S28" s="11">
         <f>R28</f>
-        <v>-1.166900834583948</v>
+        <v>1.2764220823632126</v>
       </c>
       <c r="T28" s="98" t="str">
         <f t="shared" si="13"/>
@@ -6170,11 +6203,11 @@
       </c>
       <c r="AG28" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$Q28,BID)-R28)</f>
-        <v>2.4433072145839478</v>
+        <v>1.5702363212577453E-5</v>
       </c>
       <c r="AH28" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$Q28,ASK)-S28)</f>
-        <v>2.4433072145839478</v>
+        <v>1.5702363212577453E-5</v>
       </c>
       <c r="AI28" s="84">
         <f>ABS(_xll.RtGet(SourceAlias,$U28,BID)-V28)</f>
@@ -6265,11 +6298,11 @@
       </c>
       <c r="R29" s="13">
         <f>'6M Pricing'!I29*100</f>
-        <v>-1.2194120526202104</v>
+        <v>1.2904779468119114</v>
       </c>
       <c r="S29" s="13">
         <f t="shared" si="7"/>
-        <v>-1.2194120526202104</v>
+        <v>1.2904779468119114</v>
       </c>
       <c r="T29" s="99" t="str">
         <f t="shared" si="13"/>
@@ -6324,11 +6357,11 @@
       </c>
       <c r="AG29" s="86">
         <f>ABS(_xll.RtGet(SourceAlias,$Q29,BID)-R29)</f>
-        <v>2.5098736766202103</v>
+        <v>1.6322811911440027E-5</v>
       </c>
       <c r="AH29" s="86">
         <f>ABS(_xll.RtGet(SourceAlias,$Q29,ASK)-S29)</f>
-        <v>2.5098736766202103</v>
+        <v>1.6322811911440027E-5</v>
       </c>
       <c r="AI29" s="86">
         <f>ABS(_xll.RtGet(SourceAlias,$U29,BID)-V29)</f>
@@ -6652,7 +6685,7 @@
       <c r="L6" s="34"/>
       <c r="M6" s="73" t="str">
         <f>_xll.qlIborIndex(,"Hibor",IF(OR(D6="ON",D6="TN",D6="SN"),"1D",IF(D6="SW","1W",D6)),0,Currency,Calendar,BDayConvention,EndOfMonth,DayCounter,YieldCurve,,Trigger)</f>
-        <v>obj_0027a#0000</v>
+        <v>obj_00196#0000</v>
       </c>
       <c r="N6" s="70"/>
       <c r="O6" s="72" t="b">
@@ -6701,7 +6734,7 @@
       <c r="L7" s="34"/>
       <c r="M7" s="24" t="str">
         <f>_xll.qlIborIndex(,"Hibor",IF(OR(D7="ON",D7="TN",D7="SN"),"1D",IF(D7="SW","1W",D7)),SettlementDays,Currency,Calendar,BDayConvention,EndOfMonth,DayCounter,YieldCurve,,Trigger)</f>
-        <v>obj_0027c#0000</v>
+        <v>obj_001a6#0000</v>
       </c>
       <c r="N7" s="70"/>
       <c r="O7" s="74"/>
@@ -6744,7 +6777,7 @@
       <c r="L8" s="34"/>
       <c r="M8" s="24" t="str">
         <f>_xll.qlIborIndex(,"Hibor",IF(OR(D8="ON",D8="TN",D8="SN"),"1D",IF(D8="SW","1W",D8)),SettlementDays,Currency,Calendar,BDayConvention,EndOfMonth,DayCounter,YieldCurve,,Trigger)</f>
-        <v>obj_00277#0000</v>
+        <v>obj_001a9#0000</v>
       </c>
       <c r="N8" s="70"/>
       <c r="O8" s="74"/>
@@ -6787,7 +6820,7 @@
       <c r="L9" s="34"/>
       <c r="M9" s="100" t="str">
         <f>_xll.qlIborIndex(,"Hibor",IF(OR(D9="ON",D9="TN",D9="SN"),"1D",IF(D9="SW","1W",D9)),SettlementDays,Currency,Calendar,BDayConvention,EndOfMonth,DayCounter,YieldCurve,,Trigger)</f>
-        <v>obj_0027f#0000</v>
+        <v>obj_001a3#0000</v>
       </c>
       <c r="N9" s="70"/>
       <c r="O9" s="74"/>
@@ -6859,7 +6892,7 @@
       <c r="L11" s="34"/>
       <c r="M11" s="73" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D11,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_00271#0000</v>
+        <v>obj_0019b#0000</v>
       </c>
       <c r="N11" s="34"/>
       <c r="O11" s="72" t="s">
@@ -6905,7 +6938,7 @@
       <c r="L12" s="34"/>
       <c r="M12" s="24" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D12,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_00275#0000</v>
+        <v>obj_001a4#0000</v>
       </c>
       <c r="N12" s="34"/>
       <c r="O12" s="74"/>
@@ -6945,7 +6978,7 @@
       <c r="L13" s="34"/>
       <c r="M13" s="24" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D13,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_00273#0000</v>
+        <v>obj_00198#0000</v>
       </c>
       <c r="N13" s="34"/>
       <c r="O13" s="74"/>
@@ -6988,7 +7021,7 @@
       <c r="L14" s="34"/>
       <c r="M14" s="24" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D14,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_00272#0000</v>
+        <v>obj_001a2#0000</v>
       </c>
       <c r="N14" s="34"/>
       <c r="O14" s="74"/>
@@ -7028,7 +7061,7 @@
       <c r="L15" s="34"/>
       <c r="M15" s="24" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D15,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_0027b#0000</v>
+        <v>obj_0019f#0000</v>
       </c>
       <c r="N15" s="34"/>
       <c r="O15" s="74"/>
@@ -7068,7 +7101,7 @@
       <c r="L16" s="34"/>
       <c r="M16" s="24" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D16,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_00280#0000</v>
+        <v>obj_0019d#0000</v>
       </c>
       <c r="N16" s="34"/>
       <c r="O16" s="74"/>
@@ -7111,7 +7144,7 @@
       <c r="L17" s="34"/>
       <c r="M17" s="24" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D17,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_00279#0000</v>
+        <v>obj_001ac#0000</v>
       </c>
       <c r="N17" s="70"/>
       <c r="O17" s="74"/>
@@ -7151,7 +7184,7 @@
       <c r="L18" s="34"/>
       <c r="M18" s="24" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D18,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_0026b#0000</v>
+        <v>obj_001a7#0000</v>
       </c>
       <c r="N18" s="70"/>
       <c r="O18" s="74"/>
@@ -7191,7 +7224,7 @@
       <c r="L19" s="34"/>
       <c r="M19" s="24" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D19,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_0027d#0000</v>
+        <v>obj_001aa#0000</v>
       </c>
       <c r="N19" s="70"/>
       <c r="O19" s="74"/>
@@ -7234,7 +7267,7 @@
       <c r="L20" s="34"/>
       <c r="M20" s="24" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D20,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_0026e#0000</v>
+        <v>obj_001ab#0000</v>
       </c>
       <c r="N20" s="70"/>
       <c r="O20" s="74"/>
@@ -7274,7 +7307,7 @@
       <c r="L21" s="106"/>
       <c r="M21" s="107" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D21,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_00270#0000</v>
+        <v>obj_0019e#0000</v>
       </c>
       <c r="N21" s="70"/>
       <c r="O21" s="74"/>
@@ -7317,7 +7350,7 @@
       <c r="L22" s="106"/>
       <c r="M22" s="107" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D22,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_00274#0000</v>
+        <v>obj_00199#0000</v>
       </c>
       <c r="N22" s="70"/>
       <c r="O22" s="74"/>
@@ -7360,7 +7393,7 @@
       <c r="L23" s="106"/>
       <c r="M23" s="107" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D23,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_0026d#0000</v>
+        <v>obj_0019a#0000</v>
       </c>
       <c r="N23" s="70"/>
       <c r="O23" s="74"/>
@@ -7403,7 +7436,7 @@
       <c r="L24" s="106"/>
       <c r="M24" s="107" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D24,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_0026c#0000</v>
+        <v>obj_00197#0000</v>
       </c>
       <c r="N24" s="70"/>
       <c r="O24" s="74"/>
@@ -7446,7 +7479,7 @@
       <c r="L25" s="106"/>
       <c r="M25" s="107" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D25,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_0026f#0000</v>
+        <v>obj_001a0#0000</v>
       </c>
       <c r="N25" s="70"/>
       <c r="O25" s="74"/>
@@ -7489,7 +7522,7 @@
       <c r="L26" s="106"/>
       <c r="M26" s="107" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D26,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_0026a#0000</v>
+        <v>obj_001a8#0000</v>
       </c>
       <c r="N26" s="70"/>
       <c r="O26" s="74"/>
@@ -7532,7 +7565,7 @@
       <c r="L27" s="106"/>
       <c r="M27" s="107" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D27,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_00278#0000</v>
+        <v>obj_001a1#0000</v>
       </c>
       <c r="N27" s="70"/>
       <c r="O27" s="74"/>
@@ -7575,7 +7608,7 @@
       <c r="L28" s="106"/>
       <c r="M28" s="107" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D28,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_0027e#0000</v>
+        <v>obj_001a5#0000</v>
       </c>
       <c r="N28" s="70"/>
       <c r="O28" s="74"/>
@@ -7618,7 +7651,7 @@
       <c r="L29" s="106"/>
       <c r="M29" s="116" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D29,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_00276#0000</v>
+        <v>obj_0019c#0000</v>
       </c>
       <c r="N29" s="70"/>
       <c r="O29" s="74"/>
@@ -8028,7 +8061,7 @@
       <c r="L6" s="34"/>
       <c r="M6" s="73" t="str">
         <f>_xll.qlIborIndex(,"Hibor",IF(OR(D6="ON",D6="TN",D6="SN"),"1D",IF(D6="SW","1W",D6)),0,Currency,Calendar,BDayConvention,EndOfMonth,DayCounter,YieldCurve,,Trigger)</f>
-        <v>obj_00257#0000</v>
+        <v>obj_00175#0000</v>
       </c>
       <c r="N6" s="70"/>
       <c r="O6" s="72" t="b">
@@ -8077,7 +8110,7 @@
       <c r="L7" s="34"/>
       <c r="M7" s="24" t="str">
         <f>_xll.qlIborIndex(,"Hibor",IF(OR(D7="ON",D7="TN",D7="SN"),"1D",IF(D7="SW","1W",D7)),SettlementDays,Currency,Calendar,BDayConvention,EndOfMonth,DayCounter,YieldCurve,,Trigger)</f>
-        <v>obj_0023a#0000</v>
+        <v>obj_0018c#0000</v>
       </c>
       <c r="N7" s="70"/>
       <c r="O7" s="74"/>
@@ -8120,7 +8153,7 @@
       <c r="L8" s="34"/>
       <c r="M8" s="24" t="str">
         <f>_xll.qlIborIndex(,"Hibor",IF(OR(D8="ON",D8="TN",D8="SN"),"1D",IF(D8="SW","1W",D8)),SettlementDays,Currency,Calendar,BDayConvention,EndOfMonth,DayCounter,YieldCurve,,Trigger)</f>
-        <v>obj_0024e#0000</v>
+        <v>obj_00186#0000</v>
       </c>
       <c r="N8" s="70"/>
       <c r="O8" s="74"/>
@@ -8163,7 +8196,7 @@
       <c r="L9" s="34"/>
       <c r="M9" s="24" t="str">
         <f>_xll.qlIborIndex(,"Hibor",IF(OR(D9="ON",D9="TN",D9="SN"),"1D",IF(D9="SW","1W",D9)),SettlementDays,Currency,Calendar,BDayConvention,EndOfMonth,DayCounter,YieldCurve,,Trigger)</f>
-        <v>obj_0025e#0000</v>
+        <v>obj_00178#0000</v>
       </c>
       <c r="N9" s="70"/>
       <c r="O9" s="74"/>
@@ -8203,7 +8236,7 @@
       <c r="L10" s="34"/>
       <c r="M10" s="24" t="str">
         <f>_xll.qlIborIndex(,"Hibor",IF(OR(D10="ON",D10="TN",D10="SN"),"1D",IF(D10="SW","1W",D10)),SettlementDays,Currency,Calendar,BDayConvention,EndOfMonth,DayCounter,YieldCurve,,Trigger)</f>
-        <v>obj_00239#0000</v>
+        <v>obj_0018a#0000</v>
       </c>
       <c r="N10" s="70"/>
       <c r="O10" s="74"/>
@@ -8246,7 +8279,7 @@
       <c r="L11" s="34"/>
       <c r="M11" s="26" t="str">
         <f>_xll.qlIborIndex(,"Hibor",IF(OR(D11="ON",D11="TN",D11="SN"),"1D",IF(D11="SW","1W",D11)),SettlementDays,Currency,Calendar,BDayConvention,EndOfMonth,DayCounter,YieldCurve,,Trigger)</f>
-        <v>obj_00244#0000</v>
+        <v>obj_0017a#0000</v>
       </c>
       <c r="N11" s="34"/>
       <c r="O11" s="74"/>
@@ -8634,7 +8667,7 @@
       <c r="L20" s="106"/>
       <c r="M20" s="107" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D20,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_00232#0000</v>
+        <v>obj_00164#0000</v>
       </c>
       <c r="N20" s="70"/>
       <c r="O20" s="72" t="s">
@@ -8683,7 +8716,7 @@
       <c r="L21" s="106"/>
       <c r="M21" s="107" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D21,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_0025a#0000</v>
+        <v>obj_00191#0000</v>
       </c>
       <c r="N21" s="70"/>
       <c r="O21" s="74"/>
@@ -8726,7 +8759,7 @@
       <c r="L22" s="106"/>
       <c r="M22" s="107" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D22,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_00253#0000</v>
+        <v>obj_00184#0000</v>
       </c>
       <c r="N22" s="70"/>
       <c r="O22" s="74"/>
@@ -8769,7 +8802,7 @@
       <c r="L23" s="106"/>
       <c r="M23" s="107" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D23,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_00242#0000</v>
+        <v>obj_0017c#0000</v>
       </c>
       <c r="N23" s="70"/>
       <c r="O23" s="74"/>
@@ -8812,7 +8845,7 @@
       <c r="L24" s="106"/>
       <c r="M24" s="107" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D24,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_00255#0000</v>
+        <v>obj_0017f#0000</v>
       </c>
       <c r="N24" s="70"/>
       <c r="O24" s="74"/>
@@ -8855,7 +8888,7 @@
       <c r="L25" s="106"/>
       <c r="M25" s="107" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D25,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_00254#0000</v>
+        <v>obj_00188#0000</v>
       </c>
       <c r="N25" s="70"/>
       <c r="O25" s="74"/>
@@ -8898,7 +8931,7 @@
       <c r="L26" s="106"/>
       <c r="M26" s="107" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D26,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_00243#0000</v>
+        <v>obj_00161#0000</v>
       </c>
       <c r="N26" s="70"/>
       <c r="O26" s="74"/>
@@ -8941,7 +8974,7 @@
       <c r="L27" s="106"/>
       <c r="M27" s="107" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D27,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_0023c#0000</v>
+        <v>obj_0016d#0000</v>
       </c>
       <c r="N27" s="70"/>
       <c r="O27" s="74"/>
@@ -8984,7 +9017,7 @@
       <c r="L28" s="106"/>
       <c r="M28" s="107" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D28,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_0023f#0000</v>
+        <v>obj_00179#0000</v>
       </c>
       <c r="N28" s="70"/>
       <c r="O28" s="74"/>
@@ -9027,7 +9060,7 @@
       <c r="L29" s="106"/>
       <c r="M29" s="116" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D29,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_0023e#0000</v>
+        <v>obj_00187#0000</v>
       </c>
       <c r="N29" s="70"/>
       <c r="O29" s="74"/>
@@ -9334,7 +9367,7 @@
       </c>
       <c r="I6" s="44">
         <f>_xll.qlIndexFixing(M6,F6,TRUE,AllTriggers)</f>
-        <v>1.6790870699831355E-2</v>
+        <v>5.4796902249213781E-3</v>
       </c>
       <c r="J6" s="45" t="str">
         <f>Contribution!Q6</f>
@@ -9344,7 +9377,7 @@
       <c r="L6" s="34"/>
       <c r="M6" s="73" t="str">
         <f>_xll.qlIborIndex(,"Hibor",IF(OR(D6="ON",D6="TN",D6="SN"),"1D",IF(D6="SW","1W",D6)),0,Currency,Calendar,BDayConvention,EndOfMonth,DayCounter,YieldCurve,,Trigger)</f>
-        <v>obj_00236#0000</v>
+        <v>obj_0017b#0000</v>
       </c>
       <c r="N6" s="70"/>
       <c r="O6" s="72" t="b">
@@ -9383,7 +9416,7 @@
       </c>
       <c r="I7" s="40">
         <f>_xll.qlIndexFixing(M7,F7,TRUE,AllTriggers)</f>
-        <v>1.6749878481790832E-2</v>
+        <v>5.480303076434513E-3</v>
       </c>
       <c r="J7" s="31" t="str">
         <f>Contribution!Q7</f>
@@ -9393,7 +9426,7 @@
       <c r="L7" s="34"/>
       <c r="M7" s="24" t="str">
         <f>_xll.qlIborIndex(,"Hibor",IF(OR(D7="ON",D7="TN",D7="SN"),"1D",IF(D7="SW","1W",D7)),SettlementDays,Currency,Calendar,BDayConvention,EndOfMonth,DayCounter,YieldCurve,,Trigger)</f>
-        <v>obj_00250#0000</v>
+        <v>obj_00190#0000</v>
       </c>
       <c r="N7" s="70"/>
       <c r="O7" s="74"/>
@@ -9426,7 +9459,7 @@
       </c>
       <c r="I8" s="40">
         <f>_xll.qlIndexFixing(M8,F8,TRUE,AllTriggers)</f>
-        <v>1.6683833065945865E-2</v>
+        <v>5.4813153550408479E-3</v>
       </c>
       <c r="J8" s="31" t="str">
         <f>Contribution!Q8</f>
@@ -9436,7 +9469,7 @@
       <c r="L8" s="34"/>
       <c r="M8" s="24" t="str">
         <f>_xll.qlIborIndex(,"Hibor",IF(OR(D8="ON",D8="TN",D8="SN"),"1D",IF(D8="SW","1W",D8)),SettlementDays,Currency,Calendar,BDayConvention,EndOfMonth,DayCounter,YieldCurve,,Trigger)</f>
-        <v>obj_0023b#0000</v>
+        <v>obj_0015e#0000</v>
       </c>
       <c r="N8" s="70"/>
       <c r="O8" s="74"/>
@@ -9469,7 +9502,7 @@
       </c>
       <c r="I9" s="40">
         <f>_xll.qlIndexFixing(M9,F9,TRUE,AllTriggers)</f>
-        <v>1.6389613010210823E-2</v>
+        <v>5.4851820040111646E-3</v>
       </c>
       <c r="J9" s="31" t="str">
         <f>Contribution!Q9</f>
@@ -9479,7 +9512,7 @@
       <c r="L9" s="34"/>
       <c r="M9" s="24" t="str">
         <f>_xll.qlIborIndex(,"Hibor",IF(OR(D9="ON",D9="TN",D9="SN"),"1D",IF(D9="SW","1W",D9)),SettlementDays,Currency,Calendar,BDayConvention,EndOfMonth,DayCounter,YieldCurve,,Trigger)</f>
-        <v>obj_0025d#0000</v>
+        <v>obj_00163#0000</v>
       </c>
       <c r="N9" s="70"/>
       <c r="O9" s="74"/>
@@ -9512,7 +9545,7 @@
       </c>
       <c r="I10" s="40">
         <f>_xll.qlIndexFixing(M10,F10,TRUE,AllTriggers)</f>
-        <v>1.5320304902725596E-2</v>
+        <v>5.49787709727573E-3</v>
       </c>
       <c r="J10" s="31" t="str">
         <f>Contribution!Q10</f>
@@ -9522,7 +9555,7 @@
       <c r="L10" s="34"/>
       <c r="M10" s="24" t="str">
         <f>_xll.qlIborIndex(,"Hibor",IF(OR(D10="ON",D10="TN",D10="SN"),"1D",IF(D10="SW","1W",D10)),SettlementDays,Currency,Calendar,BDayConvention,EndOfMonth,DayCounter,YieldCurve,,Trigger)</f>
-        <v>obj_00241#0000</v>
+        <v>obj_0015f#0000</v>
       </c>
       <c r="N10" s="70"/>
       <c r="O10" s="74"/>
@@ -9555,7 +9588,7 @@
       </c>
       <c r="I11" s="40">
         <f>_xll.qlIndexFixing(M11,F11,TRUE,AllTriggers)</f>
-        <v>1.3768217292016268E-2</v>
+        <v>5.5155003031810874E-3</v>
       </c>
       <c r="J11" s="31" t="str">
         <f>Contribution!Q11</f>
@@ -9565,7 +9598,7 @@
       <c r="L11" s="34"/>
       <c r="M11" s="24" t="str">
         <f>_xll.qlIborIndex(,"Hibor",IF(OR(D11="ON",D11="TN",D11="SN"),"1D",IF(D11="SW","1W",D11)),SettlementDays,Currency,Calendar,BDayConvention,EndOfMonth,DayCounter,YieldCurve,,Trigger)</f>
-        <v>obj_0023d#0000</v>
+        <v>obj_00171#0000</v>
       </c>
       <c r="N11" s="34"/>
       <c r="O11" s="74"/>
@@ -9598,7 +9631,7 @@
       </c>
       <c r="I12" s="40">
         <f>_xll.qlIndexFixing(M12,F12,TRUE,AllTriggers)</f>
-        <v>1.1495185398286246E-2</v>
+        <v>5.5407809823303086E-3</v>
       </c>
       <c r="J12" s="31" t="str">
         <f>Contribution!Q12</f>
@@ -9608,7 +9641,7 @@
       <c r="L12" s="34"/>
       <c r="M12" s="24" t="str">
         <f>_xll.qlIborIndex(,"Hibor",IF(OR(D12="ON",D12="TN",D12="SN"),"1D",IF(D12="SW","1W",D12)),SettlementDays,Currency,Calendar,BDayConvention,EndOfMonth,DayCounter,YieldCurve,,Trigger)</f>
-        <v>obj_00234#0000</v>
+        <v>obj_00169#0000</v>
       </c>
       <c r="N12" s="34"/>
       <c r="O12" s="74"/>
@@ -9641,7 +9674,7 @@
       </c>
       <c r="I13" s="40">
         <f>_xll.qlIndexFixing(M13,F13,TRUE,AllTriggers)</f>
-        <v>8.5884049460434372E-3</v>
+        <v>5.572727924082599E-3</v>
       </c>
       <c r="J13" s="31" t="str">
         <f>Contribution!Q13</f>
@@ -9651,7 +9684,7 @@
       <c r="L13" s="34"/>
       <c r="M13" s="24" t="str">
         <f>_xll.qlIborIndex(,"Hibor",IF(OR(D13="ON",D13="TN",D13="SN"),"1D",IF(D13="SW","1W",D13)),SettlementDays,Currency,Calendar,BDayConvention,EndOfMonth,DayCounter,YieldCurve,,Trigger)</f>
-        <v>obj_00237#0000</v>
+        <v>obj_00182#0000</v>
       </c>
       <c r="N13" s="34"/>
       <c r="O13" s="74"/>
@@ -9684,7 +9717,7 @@
       </c>
       <c r="I14" s="43">
         <f>_xll.qlIndexFixing(M14,F14,TRUE,AllTriggers)</f>
-        <v>5.2952602541179276E-3</v>
+        <v>5.6086587043454343E-3</v>
       </c>
       <c r="J14" s="33" t="str">
         <f>Contribution!Q14</f>
@@ -9694,7 +9727,7 @@
       <c r="L14" s="34"/>
       <c r="M14" s="26" t="str">
         <f>_xll.qlIborIndex(,"Hibor",IF(OR(D14="ON",D14="TN",D14="SN"),"1D",IF(D14="SW","1W",D14)),SettlementDays,Currency,Calendar,BDayConvention,EndOfMonth,DayCounter,YieldCurve,,Trigger)</f>
-        <v>obj_00246#0000</v>
+        <v>obj_00160#0000</v>
       </c>
       <c r="N14" s="34"/>
       <c r="O14" s="74"/>
@@ -9731,7 +9764,7 @@
       </c>
       <c r="I15" s="39">
         <f>_xll.qlIndexFixing(IborIndex,F15,TRUE,AllTriggers)</f>
-        <v>-3.2640991011183209E-4</v>
+        <v>5.7186023228693057E-3</v>
       </c>
       <c r="J15" s="32" t="str">
         <f>Contribution!Q15</f>
@@ -9775,7 +9808,7 @@
       </c>
       <c r="I16" s="40">
         <f>_xll.qlIndexFixing(IborIndex,F16,TRUE,AllTriggers)</f>
-        <v>1.0397867244255035E-4</v>
+        <v>6.0837988335763786E-3</v>
       </c>
       <c r="J16" s="31" t="str">
         <f>Contribution!Q16</f>
@@ -9819,7 +9852,7 @@
       </c>
       <c r="I17" s="40">
         <f>_xll.qlIndexFixing(IborIndex,F17,TRUE,AllTriggers)</f>
-        <v>-9.5927591562247224E-6</v>
+        <v>6.6332620453451582E-3</v>
       </c>
       <c r="J17" s="31" t="str">
         <f>Contribution!Q17</f>
@@ -9863,7 +9896,7 @@
       </c>
       <c r="I18" s="40">
         <f>_xll.qlIndexFixing(IborIndex,F18,TRUE,AllTriggers)</f>
-        <v>6.0833558678996898E-6</v>
+        <v>7.0796198639139643E-3</v>
       </c>
       <c r="J18" s="31" t="str">
         <f>Contribution!Q18</f>
@@ -9907,7 +9940,7 @@
       </c>
       <c r="I19" s="40">
         <f>_xll.qlIndexFixing(IborIndex,F19,TRUE,AllTriggers)</f>
-        <v>2.0201377357025946E-5</v>
+        <v>7.4621169541505966E-3</v>
       </c>
       <c r="J19" s="31" t="str">
         <f>Contribution!Q19</f>
@@ -9951,7 +9984,7 @@
       </c>
       <c r="I20" s="88">
         <f>_xll.qlIndexFixing(IborIndex,F20,TRUE,AllTriggers)</f>
-        <v>-3.5271658559814796E-5</v>
+        <v>7.8265007100070012E-3</v>
       </c>
       <c r="J20" s="47" t="str">
         <f>Contribution!Q20</f>
@@ -9995,7 +10028,7 @@
       </c>
       <c r="I21" s="88">
         <f>_xll.qlIndexFixing(IborIndex,F21,TRUE,AllTriggers)</f>
-        <v>-7.4190239538407043E-6</v>
+        <v>1.0544016682418925E-2</v>
       </c>
       <c r="J21" s="47" t="str">
         <f>Contribution!Q21</f>
@@ -10039,7 +10072,7 @@
       </c>
       <c r="I22" s="114">
         <f>_xll.qlIndexFixing(IborIndex,F22,TRUE,AllTriggers)</f>
-        <v>1.2203135604930688E-4</v>
+        <v>1.3120611247400937E-2</v>
       </c>
       <c r="J22" s="115" t="str">
         <f>Contribution!Q22</f>
@@ -10087,7 +10120,7 @@
       </c>
       <c r="I23" s="88">
         <f>_xll.qlIndexFixing(M23,F23,TRUE,AllTriggers)</f>
-        <v>-3.8335737215488041E-3</v>
+        <v>1.0653784599269873E-2</v>
       </c>
       <c r="J23" s="47" t="str">
         <f>Contribution!Q23</f>
@@ -10097,7 +10130,7 @@
       <c r="L23" s="106"/>
       <c r="M23" s="107" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D23,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_00258#0000</v>
+        <v>obj_00167#0000</v>
       </c>
       <c r="N23" s="70"/>
       <c r="O23" s="72" t="s">
@@ -10136,7 +10169,7 @@
       </c>
       <c r="I24" s="88">
         <f>_xll.qlIndexFixing(M24,F24,TRUE,AllTriggers)</f>
-        <v>-6.4461427424037775E-3</v>
+        <v>1.1360400410021657E-2</v>
       </c>
       <c r="J24" s="47" t="str">
         <f>Contribution!Q24</f>
@@ -10146,7 +10179,7 @@
       <c r="L24" s="106"/>
       <c r="M24" s="107" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D24,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_00235#0000</v>
+        <v>obj_0016c#0000</v>
       </c>
       <c r="N24" s="70"/>
       <c r="O24" s="74"/>
@@ -10179,7 +10212,7 @@
       </c>
       <c r="I25" s="88">
         <f>_xll.qlIndexFixing(M25,F25,TRUE,AllTriggers)</f>
-        <v>-8.0048840792654227E-3</v>
+        <v>1.1780535604938695E-2</v>
       </c>
       <c r="J25" s="47" t="str">
         <f>Contribution!Q25</f>
@@ -10189,7 +10222,7 @@
       <c r="L25" s="106"/>
       <c r="M25" s="107" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D25,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_00247#0000</v>
+        <v>obj_0017d#0000</v>
       </c>
       <c r="N25" s="70"/>
       <c r="O25" s="74"/>
@@ -10222,7 +10255,7 @@
       </c>
       <c r="I26" s="88">
         <f>_xll.qlIndexFixing(M26,F26,TRUE,AllTriggers)</f>
-        <v>-9.7971275502906872E-3</v>
+        <v>1.2262374872902439E-2</v>
       </c>
       <c r="J26" s="47" t="str">
         <f>Contribution!Q26</f>
@@ -10232,7 +10265,7 @@
       <c r="L26" s="106"/>
       <c r="M26" s="107" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D26,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_0024f#0000</v>
+        <v>obj_00166#0000</v>
       </c>
       <c r="N26" s="70"/>
       <c r="O26" s="74"/>
@@ -10265,7 +10298,7 @@
       </c>
       <c r="I27" s="88">
         <f>_xll.qlIndexFixing(M27,F27,TRUE,AllTriggers)</f>
-        <v>-1.1145863978438648E-2</v>
+        <v>1.2624128360856059E-2</v>
       </c>
       <c r="J27" s="47" t="str">
         <f>Contribution!Q27</f>
@@ -10275,7 +10308,7 @@
       <c r="L27" s="106"/>
       <c r="M27" s="107" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D27,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_0024c#0000</v>
+        <v>obj_0018f#0000</v>
       </c>
       <c r="N27" s="70"/>
       <c r="O27" s="74"/>
@@ -10308,7 +10341,7 @@
       </c>
       <c r="I28" s="88">
         <f>_xll.qlIndexFixing(M28,F28,TRUE,AllTriggers)</f>
-        <v>-1.166900834583948E-2</v>
+        <v>1.2764220823632126E-2</v>
       </c>
       <c r="J28" s="47" t="str">
         <f>Contribution!Q28</f>
@@ -10318,7 +10351,7 @@
       <c r="L28" s="106"/>
       <c r="M28" s="107" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D28,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_00240#0000</v>
+        <v>obj_0018d#0000</v>
       </c>
       <c r="N28" s="70"/>
       <c r="O28" s="74"/>
@@ -10351,7 +10384,7 @@
       </c>
       <c r="I29" s="114">
         <f>_xll.qlIndexFixing(M29,F29,TRUE,AllTriggers)</f>
-        <v>-1.2194120526202104E-2</v>
+        <v>1.2904779468119115E-2</v>
       </c>
       <c r="J29" s="115" t="str">
         <f>Contribution!Q29</f>
@@ -10361,7 +10394,7 @@
       <c r="L29" s="106"/>
       <c r="M29" s="116" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D29,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_0024a#0000</v>
+        <v>obj_00177#0000</v>
       </c>
       <c r="N29" s="70"/>
       <c r="O29" s="74"/>
@@ -10572,7 +10605,7 @@
       <c r="K3" s="74"/>
       <c r="M3" s="26" t="str">
         <f>_xll.qlOvernightIndex(,"Honix",0,Currency,Calendar,"act/365 (fixed)",YieldCurve,,Trigger)</f>
-        <v>obj_0024d#0000</v>
+        <v>obj_00162#0000</v>
       </c>
       <c r="O3" s="74"/>
       <c r="P3" s="74"/>
@@ -10677,7 +10710,7 @@
       <c r="L6" s="34"/>
       <c r="M6" s="107" t="str">
         <f>_xll.qlMakeOIS(,SettlementDays,IF(D6="ON","1D",D6),OvernightIndex,,ForwardStart,FixedLegDayCounter,,,Trigger)</f>
-        <v>obj_00263#0000</v>
+        <v>obj_00194#0000</v>
       </c>
       <c r="N6" s="70"/>
       <c r="O6" s="72" t="s">
@@ -10723,7 +10756,7 @@
       <c r="L7" s="34"/>
       <c r="M7" s="107" t="str">
         <f>_xll.qlMakeOIS(,SettlementDays,IF(D7="ON","1D",D7),OvernightIndex,,ForwardStart,FixedLegDayCounter,,,Trigger)</f>
-        <v>obj_00269#0000</v>
+        <v>obj_00193#0000</v>
       </c>
       <c r="N7" s="70"/>
       <c r="O7" s="74"/>
@@ -10761,7 +10794,7 @@
       <c r="L8" s="34"/>
       <c r="M8" s="107" t="str">
         <f>_xll.qlMakeOIS(,SettlementDays,IF(D8="ON","1D",D8),OvernightIndex,,ForwardStart,FixedLegDayCounter,,,Trigger)</f>
-        <v>obj_00260#0000</v>
+        <v>obj_00185#0000</v>
       </c>
       <c r="N8" s="70"/>
       <c r="O8" s="74"/>
@@ -10802,7 +10835,7 @@
       <c r="L9" s="34"/>
       <c r="M9" s="107" t="str">
         <f>_xll.qlMakeOIS(,SettlementDays,IF(D9="ON","1D",D9),OvernightIndex,,ForwardStart,FixedLegDayCounter,,,Trigger)</f>
-        <v>obj_00259#0000</v>
+        <v>obj_0016a#0000</v>
       </c>
       <c r="N9" s="70"/>
       <c r="O9" s="74"/>
@@ -10843,7 +10876,7 @@
       <c r="L10" s="34"/>
       <c r="M10" s="107" t="str">
         <f>_xll.qlMakeOIS(,SettlementDays,IF(D10="ON","1D",D10),OvernightIndex,,ForwardStart,FixedLegDayCounter,,,Trigger)</f>
-        <v>obj_00261#0000</v>
+        <v>obj_00189#0000</v>
       </c>
       <c r="N10" s="70"/>
       <c r="O10" s="74"/>
@@ -10884,7 +10917,7 @@
       <c r="L11" s="34"/>
       <c r="M11" s="107" t="str">
         <f>_xll.qlMakeOIS(,SettlementDays,IF(D11="ON","1D",D11),OvernightIndex,,ForwardStart,FixedLegDayCounter,,,Trigger)</f>
-        <v>obj_00267#0000</v>
+        <v>obj_00168#0000</v>
       </c>
       <c r="N11" s="70"/>
       <c r="O11" s="74"/>
@@ -10925,7 +10958,7 @@
       <c r="L12" s="34"/>
       <c r="M12" s="107" t="str">
         <f>_xll.qlMakeOIS(,SettlementDays,IF(D12="ON","1D",D12),OvernightIndex,,ForwardStart,FixedLegDayCounter,,,Trigger)</f>
-        <v>obj_00268#0000</v>
+        <v>obj_0016b#0000</v>
       </c>
       <c r="N12" s="70"/>
       <c r="O12" s="74"/>
@@ -10966,7 +10999,7 @@
       <c r="L13" s="34"/>
       <c r="M13" s="107" t="str">
         <f>_xll.qlMakeOIS(,SettlementDays,IF(D13="ON","1D",D13),OvernightIndex,,ForwardStart,FixedLegDayCounter,,,Trigger)</f>
-        <v>obj_0025c#0000</v>
+        <v>obj_0016f#0000</v>
       </c>
       <c r="N13" s="70"/>
       <c r="O13" s="74"/>
@@ -11007,7 +11040,7 @@
       <c r="L14" s="34"/>
       <c r="M14" s="107" t="str">
         <f>_xll.qlMakeOIS(,SettlementDays,IF(D14="ON","1D",D14),OvernightIndex,,ForwardStart,FixedLegDayCounter,,,Trigger)</f>
-        <v>obj_00265#0000</v>
+        <v>obj_00181#0000</v>
       </c>
       <c r="N14" s="70"/>
       <c r="O14" s="74"/>
@@ -11045,7 +11078,7 @@
       <c r="L15" s="34"/>
       <c r="M15" s="107" t="str">
         <f>_xll.qlMakeOIS(,SettlementDays,IF(D15="ON","1D",D15),OvernightIndex,,ForwardStart,FixedLegDayCounter,,,Trigger)</f>
-        <v>obj_00256#0000</v>
+        <v>obj_00172#0000</v>
       </c>
       <c r="N15" s="70"/>
       <c r="O15" s="74"/>
@@ -11083,7 +11116,7 @@
       <c r="L16" s="34"/>
       <c r="M16" s="107" t="str">
         <f>_xll.qlMakeOIS(,SettlementDays,IF(D16="ON","1D",D16),OvernightIndex,,ForwardStart,FixedLegDayCounter,,,Trigger)</f>
-        <v>obj_00266#0000</v>
+        <v>obj_00173#0000</v>
       </c>
       <c r="N16" s="70"/>
       <c r="O16" s="74"/>
@@ -11124,7 +11157,7 @@
       <c r="L17" s="34"/>
       <c r="M17" s="107" t="str">
         <f>_xll.qlMakeOIS(,SettlementDays,IF(D17="ON","1D",D17),OvernightIndex,,ForwardStart,FixedLegDayCounter,,,Trigger)</f>
-        <v>obj_0025b#0000</v>
+        <v>obj_00195#0000</v>
       </c>
       <c r="N17" s="70"/>
       <c r="O17" s="74"/>
@@ -11162,7 +11195,7 @@
       <c r="L18" s="34"/>
       <c r="M18" s="107" t="str">
         <f>_xll.qlMakeOIS(,SettlementDays,IF(D18="ON","1D",D18),OvernightIndex,,ForwardStart,FixedLegDayCounter,,,Trigger)</f>
-        <v>obj_00264#0000</v>
+        <v>obj_00170#0000</v>
       </c>
       <c r="N18" s="70"/>
       <c r="O18" s="74"/>
@@ -11200,7 +11233,7 @@
       <c r="L19" s="34"/>
       <c r="M19" s="107" t="str">
         <f>_xll.qlMakeOIS(,SettlementDays,IF(D19="ON","1D",D19),OvernightIndex,,ForwardStart,FixedLegDayCounter,,,Trigger)</f>
-        <v>obj_0025f#0000</v>
+        <v>obj_00180#0000</v>
       </c>
       <c r="N19" s="70"/>
       <c r="O19" s="74"/>
@@ -11241,7 +11274,7 @@
       <c r="L20" s="106"/>
       <c r="M20" s="107" t="str">
         <f>_xll.qlMakeOIS(,SettlementDays,IF(D20="ON","1D",D20),OvernightIndex,,ForwardStart,FixedLegDayCounter,,,Trigger)</f>
-        <v>obj_00262#0000</v>
+        <v>obj_00192#0000</v>
       </c>
       <c r="N20" s="70"/>
       <c r="O20" s="74"/>
@@ -12311,7 +12344,7 @@
       <c r="L22" s="106"/>
       <c r="M22" s="107" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D22,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_00251#0000</v>
+        <v>obj_0016e#0000</v>
       </c>
       <c r="N22" s="70"/>
       <c r="O22" s="72" t="s">
@@ -12360,7 +12393,7 @@
       <c r="L23" s="106"/>
       <c r="M23" s="107" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D23,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_0024b#0000</v>
+        <v>obj_0018b#0000</v>
       </c>
       <c r="N23" s="70"/>
       <c r="O23" s="74"/>
@@ -12403,7 +12436,7 @@
       <c r="L24" s="106"/>
       <c r="M24" s="107" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D24,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_00245#0000</v>
+        <v>obj_0018e#0000</v>
       </c>
       <c r="N24" s="70"/>
       <c r="O24" s="74"/>
@@ -12446,7 +12479,7 @@
       <c r="L25" s="106"/>
       <c r="M25" s="107" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D25,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_00252#0000</v>
+        <v>obj_0017e#0000</v>
       </c>
       <c r="N25" s="70"/>
       <c r="O25" s="74"/>
@@ -12489,7 +12522,7 @@
       <c r="L26" s="106"/>
       <c r="M26" s="107" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D26,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_00249#0000</v>
+        <v>obj_00174#0000</v>
       </c>
       <c r="N26" s="70"/>
       <c r="O26" s="74"/>
@@ -12532,7 +12565,7 @@
       <c r="L27" s="106"/>
       <c r="M27" s="107" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D27,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_00248#0000</v>
+        <v>obj_00183#0000</v>
       </c>
       <c r="N27" s="70"/>
       <c r="O27" s="74"/>
@@ -12575,7 +12608,7 @@
       <c r="L28" s="106"/>
       <c r="M28" s="107" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D28,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_00238#0000</v>
+        <v>obj_00176#0000</v>
       </c>
       <c r="N28" s="70"/>
       <c r="O28" s="74"/>
@@ -12618,7 +12651,7 @@
       <c r="L29" s="106"/>
       <c r="M29" s="116" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D29,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_00233#0000</v>
+        <v>obj_00165#0000</v>
       </c>
       <c r="N29" s="70"/>
       <c r="O29" s="74"/>

</xml_diff>